<commit_message>
Add test for generating MC2020 with OA20251 codes and implement necessary functions
- Created `generate_malla_with_oa_codes.rs` to test the integration of OA20251 codes into MC2020 structure.
- Implemented functions to read OA20251 codes and MC2020 structure from Excel files.
- Added normalization and matching logic using Jaro-Winkler algorithm for course names.
- Generated output files in CSV and JSON formats for corrected mappings.
- Documented test results in `TEST_RESULTS_SUMMARY.md` with detailed information on execution and outcomes.
</commit_message>
<xml_diff>
--- a/quickshift/src/datafiles/MC2020.xlsx
+++ b/quickshift/src/datafiles/MC2020.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="181">
   <si>
     <t>Num Correlativo</t>
   </si>
@@ -66,7 +66,7 @@
     <t>54</t>
   </si>
   <si>
-    <t>CIT1000</t>
+    <t>CIT1010</t>
   </si>
   <si>
     <t>PROGRAMACIÓN</t>
@@ -93,7 +93,7 @@
     <t>11, 22</t>
   </si>
   <si>
-    <t>CBM1003</t>
+    <t>CBM1006</t>
   </si>
   <si>
     <t>CÁLCULO II</t>
@@ -114,9 +114,6 @@
     <t>13, 17</t>
   </si>
   <si>
-    <t>CIT1010</t>
-  </si>
-  <si>
     <t>PROGRAMACIÓN AVANZADA</t>
   </si>
   <si>
@@ -144,9 +141,6 @@
     <t>17, 18</t>
   </si>
   <si>
-    <t>CBM1006</t>
-  </si>
-  <si>
     <t>CÁLCULO III</t>
   </si>
   <si>
@@ -219,7 +213,7 @@
     <t>36</t>
   </si>
   <si>
-    <t>CIT2007</t>
+    <t>CIT2009</t>
   </si>
   <si>
     <t>BASES DE DATOS</t>
@@ -240,370 +234,328 @@
     <t>24</t>
   </si>
   <si>
+    <t>CIG1003</t>
+  </si>
+  <si>
+    <t>INGLÉS GENERAL I</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>CII2750</t>
+  </si>
+  <si>
+    <t>OPTIMIZACIÓN</t>
+  </si>
+  <si>
+    <t>6, 12</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>CIT2108</t>
+  </si>
+  <si>
+    <t>TALLER DE REDES Y SERVICIOS</t>
+  </si>
+  <si>
+    <t>15, 16</t>
+  </si>
+  <si>
+    <t>31, 41</t>
+  </si>
+  <si>
+    <t>CIT3203</t>
+  </si>
+  <si>
+    <t>PROYECTO EN TICS I</t>
+  </si>
+  <si>
+    <t>15, 20</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>BASES DE DATOS AVANZADAS</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>CFG2</t>
+  </si>
+  <si>
+    <t>CFG-2</t>
+  </si>
+  <si>
+    <t>INGLÉS GENERAL II</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>CII1000</t>
+  </si>
+  <si>
+    <t>CONTABILIDAD Y COSTOS</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>CIT2109</t>
+  </si>
+  <si>
+    <t>ARQUITECTURA Y ORGANIZ DE COMPUTADORES</t>
+  </si>
+  <si>
+    <t>15, 17</t>
+  </si>
+  <si>
+    <t>CIT2110</t>
+  </si>
+  <si>
+    <t>SEÑALES Y SISTEMAS</t>
+  </si>
+  <si>
+    <t>CIT2010</t>
+  </si>
+  <si>
+    <t>SISTEMAS OPERATIVOS</t>
+  </si>
+  <si>
+    <t>14, 23</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>CFG3</t>
+  </si>
+  <si>
+    <t>CFG-3</t>
+  </si>
+  <si>
+    <t>INGLÉS GENERAL III</t>
+  </si>
+  <si>
+    <t>CIT2206</t>
+  </si>
+  <si>
+    <t>GESTIÓN ORGANIZACIONAL</t>
+  </si>
+  <si>
+    <t>CIT2011</t>
+  </si>
+  <si>
+    <t>SISTEMAS DISTRIBUIDOS</t>
+  </si>
+  <si>
+    <t>15, 31</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>COMUNICACIONES DIGITALES</t>
+  </si>
+  <si>
+    <t>18, 30</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>CIT2012</t>
+  </si>
+  <si>
+    <t>INGENIERÍA DE SOFTWARE</t>
+  </si>
+  <si>
+    <t>19, 24</t>
+  </si>
+  <si>
+    <t>43, 47</t>
+  </si>
+  <si>
+    <t>CFG4</t>
+  </si>
+  <si>
+    <t>CFG-4</t>
+  </si>
+  <si>
+    <t>CII2100</t>
+  </si>
+  <si>
+    <t>INTRODUCCIÓN A LA ECONOMÍA</t>
+  </si>
+  <si>
+    <t>CIT2112</t>
+  </si>
+  <si>
+    <t>TECNOLOGÍAS INALÁMBRICAS</t>
+  </si>
+  <si>
+    <t>CIT2113</t>
+  </si>
+  <si>
+    <t>CRIPTOGRAFÍA Y SEGURIDAD EN REDES</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>CIT3325</t>
+  </si>
+  <si>
+    <t>INTELIGENCIA ARTIFICAL</t>
+  </si>
+  <si>
+    <t>16, 19, 22</t>
+  </si>
+  <si>
+    <t>CIT2207</t>
+  </si>
+  <si>
+    <t>EVALUACION DE PROYECTOS TIC</t>
+  </si>
+  <si>
+    <t>28, 34, 37</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>ELECTIVO PROFESIONAL INF 1</t>
+  </si>
+  <si>
+    <t>ARQUITECTURAS EMERGENTES</t>
+  </si>
+  <si>
+    <t>ELECTIVO PROFESIONAL TEL 1</t>
+  </si>
+  <si>
+    <t>ARQUITECTURA DE SOFTWARE</t>
+  </si>
+  <si>
+    <t>CIT3202</t>
+  </si>
+  <si>
+    <t>DATA SCIENCE</t>
+  </si>
+  <si>
+    <t>25, 42</t>
+  </si>
+  <si>
+    <t>ELECTIVO PROFESIONAL INF 2</t>
+  </si>
+  <si>
+    <t>ELECTIVO PROFESIONAL TEL 2</t>
+  </si>
+  <si>
+    <t>ELECTIVO PROFESIONAL TEL 3</t>
+  </si>
+  <si>
+    <t>ELECTIVO PROFESIONAL INF 3</t>
+  </si>
+  <si>
+    <t>PROYECTO EN TICS II</t>
+  </si>
+  <si>
+    <t>CIT5002</t>
+  </si>
+  <si>
+    <t>PRÁCTICA PROFESIONAL 1</t>
+  </si>
+  <si>
+    <t>3, 5, 10, 15, 16, 17, 18, 19 , 20, 21</t>
+  </si>
+  <si>
+    <t>PRÁCTICA PROFESIONAL 2</t>
+  </si>
+  <si>
+    <t>22, 25, 26, 29, 32, 33, 35, 38, 39, 40, 41, 42, 43</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Codigo</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Abre</t>
+  </si>
+  <si>
+    <t>Prerrequisito</t>
+  </si>
+  <si>
+    <t>Equivalencia</t>
+  </si>
+  <si>
+    <t>CIT3350</t>
+  </si>
+  <si>
+    <t>DATA STREAM PROCESSING</t>
+  </si>
+  <si>
+    <t>CIT2003, CIT2104, CIT2010, CIT2109</t>
+  </si>
+  <si>
+    <t>CIT3347</t>
+  </si>
+  <si>
+    <t>DIS Y DESARROLLO DE SIST INTERACTIVOS</t>
+  </si>
+  <si>
+    <t>CIT2012, CIT2005</t>
+  </si>
+  <si>
+    <t>CIT3349</t>
+  </si>
+  <si>
+    <t>GRAFOS Y ALGORITMOS</t>
+  </si>
+  <si>
+    <t>CII2750, CIT2204, CIT2007, CIT2002</t>
+  </si>
+  <si>
+    <t>INTELIGENCIA DE NEGOCIOS</t>
+  </si>
+  <si>
+    <t>CIT2005, CIT2012</t>
+  </si>
+  <si>
+    <t>CIT3348</t>
+  </si>
+  <si>
+    <t>TALLER DE TRANSFORMACIÓN DIGITAL</t>
+  </si>
+  <si>
+    <t>CIT2005, CIT3100</t>
+  </si>
+  <si>
+    <t>CIG1013</t>
+  </si>
+  <si>
     <t>CIG1012</t>
-  </si>
-  <si>
-    <t>INGLÉS GENERAL I</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>CII2750</t>
-  </si>
-  <si>
-    <t>OPTIMIZACIÓN</t>
-  </si>
-  <si>
-    <t>6, 12</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>CIT2108</t>
-  </si>
-  <si>
-    <t>TALLER DE REDES Y SERVICIOS</t>
-  </si>
-  <si>
-    <t>15, 16</t>
-  </si>
-  <si>
-    <t>31, 41</t>
-  </si>
-  <si>
-    <t>CIT2205</t>
-  </si>
-  <si>
-    <t>PROYECTO EN TICS I</t>
-  </si>
-  <si>
-    <t>15, 20</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>CIT2009</t>
-  </si>
-  <si>
-    <t>BASES DE DATOS AVANZADAS</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t>CFG2</t>
-  </si>
-  <si>
-    <t>CFG-2</t>
-  </si>
-  <si>
-    <t>CIG1013</t>
-  </si>
-  <si>
-    <t>INGLÉS GENERAL II</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>CII1000</t>
-  </si>
-  <si>
-    <t>CONTABILIDAD Y COSTOS</t>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>CIT2109</t>
-  </si>
-  <si>
-    <t>ARQUITECTURA Y ORGANIZ DE COMPUTADORES</t>
-  </si>
-  <si>
-    <t>15, 17</t>
-  </si>
-  <si>
-    <t>CIT2110</t>
-  </si>
-  <si>
-    <t>SEÑALES Y SISTEMAS</t>
-  </si>
-  <si>
-    <t>CIT2010</t>
-  </si>
-  <si>
-    <t>SISTEMAS OPERATIVOS</t>
-  </si>
-  <si>
-    <t>14, 23</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>CFG3</t>
-  </si>
-  <si>
-    <t>CFG-3</t>
-  </si>
-  <si>
-    <t>CIG1014</t>
-  </si>
-  <si>
-    <t>INGLÉS GENERAL III</t>
-  </si>
-  <si>
-    <t>CIT2206</t>
-  </si>
-  <si>
-    <t>GESTIÓN ORGANIZACIONAL</t>
-  </si>
-  <si>
-    <t>CIT2011</t>
-  </si>
-  <si>
-    <t>SISTEMAS DISTRIBUIDOS</t>
-  </si>
-  <si>
-    <t>15, 31</t>
-  </si>
-  <si>
-    <t>45</t>
-  </si>
-  <si>
-    <t>CIT2111</t>
-  </si>
-  <si>
-    <t>COMUNICACIONES DIGITALES</t>
-  </si>
-  <si>
-    <t>18, 30</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>CIT2012</t>
-  </si>
-  <si>
-    <t>INGENIERÍA DE SOFTWARE</t>
-  </si>
-  <si>
-    <t>19, 24</t>
-  </si>
-  <si>
-    <t>43, 47</t>
-  </si>
-  <si>
-    <t>CFG4</t>
-  </si>
-  <si>
-    <t>CFG-4</t>
-  </si>
-  <si>
-    <t>CII2100</t>
-  </si>
-  <si>
-    <t>INTRODUCCIÓN A LA ECONOMÍA</t>
-  </si>
-  <si>
-    <t>CIT2112</t>
-  </si>
-  <si>
-    <t>TECNOLOGÍAS INALÁMBRICAS</t>
-  </si>
-  <si>
-    <t>CIT2113</t>
-  </si>
-  <si>
-    <t>CRIPTOGRAFÍA Y SEGURIDAD EN REDES</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>CIT2013</t>
-  </si>
-  <si>
-    <t>INTELIGENCIA ARTIFICAL</t>
-  </si>
-  <si>
-    <t>16, 19, 22</t>
-  </si>
-  <si>
-    <t>CIT2207</t>
-  </si>
-  <si>
-    <t>EVALUACION DE PROYECTOS TIC</t>
-  </si>
-  <si>
-    <t>28, 34, 37</t>
-  </si>
-  <si>
-    <t>53</t>
-  </si>
-  <si>
-    <t>CIT3310</t>
-  </si>
-  <si>
-    <t>ELECTIVO PROFESIONAL INF 1</t>
-  </si>
-  <si>
-    <t>CIT3100</t>
-  </si>
-  <si>
-    <t>ARQUITECTURAS EMERGENTES</t>
-  </si>
-  <si>
-    <t>CIT3410</t>
-  </si>
-  <si>
-    <t>ELECTIVO PROFESIONAL TEL 1</t>
-  </si>
-  <si>
-    <t>CIT3000</t>
-  </si>
-  <si>
-    <t>ARQUITECTURA DE SOFTWARE</t>
-  </si>
-  <si>
-    <t>CIT3202</t>
-  </si>
-  <si>
-    <t>DATA SCIENCE</t>
-  </si>
-  <si>
-    <t>25, 42</t>
-  </si>
-  <si>
-    <t>CIT3311</t>
-  </si>
-  <si>
-    <t>ELECTIVO PROFESIONAL INF 2</t>
-  </si>
-  <si>
-    <t>CIT3411</t>
-  </si>
-  <si>
-    <t>ELECTIVO PROFESIONAL TEL 2</t>
-  </si>
-  <si>
-    <t>CIT3412</t>
-  </si>
-  <si>
-    <t>ELECTIVO PROFESIONAL TEL 3</t>
-  </si>
-  <si>
-    <t>CIT3312</t>
-  </si>
-  <si>
-    <t>ELECTIVO PROFESIONAL INF 3</t>
-  </si>
-  <si>
-    <t>CIT3203</t>
-  </si>
-  <si>
-    <t>PROYECTO EN TICS II</t>
-  </si>
-  <si>
-    <t>CIT4000</t>
-  </si>
-  <si>
-    <t>PRÁCTICA PROFESIONAL 1</t>
-  </si>
-  <si>
-    <t>3, 5, 10, 15, 16, 17, 18, 19 , 20, 21</t>
-  </si>
-  <si>
-    <t>CIT4001</t>
-  </si>
-  <si>
-    <t>PRÁCTICA PROFESIONAL 2</t>
-  </si>
-  <si>
-    <t>22, 25, 26, 29, 32, 33, 35, 38, 39, 40, 41, 42, 43</t>
-  </si>
-  <si>
-    <t>Final</t>
-  </si>
-  <si>
-    <t>44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55</t>
-  </si>
-  <si>
-    <t>Tipo</t>
-  </si>
-  <si>
-    <t>Codigo</t>
-  </si>
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Abre</t>
-  </si>
-  <si>
-    <t>Prerrequisito</t>
-  </si>
-  <si>
-    <t>Equivalencia</t>
-  </si>
-  <si>
-    <t>CIT3350</t>
-  </si>
-  <si>
-    <t>DATA STREAM PROCESSING</t>
-  </si>
-  <si>
-    <t>CIT2003, CIT2104, CIT2010, CIT2109</t>
-  </si>
-  <si>
-    <t>CIT3347</t>
-  </si>
-  <si>
-    <t>DIS Y DESARROLLO DE SIST INTERACTIVOS</t>
-  </si>
-  <si>
-    <t>CIT2012, CIT2005</t>
-  </si>
-  <si>
-    <t>CIT3349</t>
-  </si>
-  <si>
-    <t>GRAFOS Y ALGORITMOS</t>
-  </si>
-  <si>
-    <t>CII2750, CIT2204, CIT2007, CIT2002</t>
-  </si>
-  <si>
-    <t>CIT3325</t>
-  </si>
-  <si>
-    <t>INTELIGENCIA DE NEGOCIOS</t>
-  </si>
-  <si>
-    <t>CIT2005, CIT2012</t>
-  </si>
-  <si>
-    <t>CIT3348</t>
-  </si>
-  <si>
-    <t>TALLER DE TRANSFORMACIÓN DIGITAL</t>
-  </si>
-  <si>
-    <t>CIT2005, CIT3100</t>
-  </si>
-  <si>
-    <t>CIG1003</t>
   </si>
   <si>
     <t>CIG1002</t>
@@ -614,12 +566,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -661,22 +613,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -690,23 +642,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -720,12 +665,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -744,22 +717,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -774,33 +732,20 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="48">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -905,181 +850,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1136,35 +1045,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1180,6 +1065,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1204,16 +1113,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -1221,144 +1130,144 @@
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="40" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1787,8 +1696,8 @@
   <sheetPr/>
   <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14166666666667" defaultRowHeight="15"/>
@@ -1987,16 +1896,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="D10" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="E10" s="37" t="s">
         <v>34</v>
-      </c>
-      <c r="E10" s="37" t="s">
-        <v>35</v>
       </c>
       <c r="F10" s="38">
         <v>2</v>
@@ -2007,10 +1916,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="18" t="s">
         <v>36</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>37</v>
       </c>
       <c r="D11" s="19" t="s">
         <v>8</v>
@@ -2027,16 +1936,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="D12" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="E12" s="39" t="s">
         <v>40</v>
-      </c>
-      <c r="E12" s="39" t="s">
-        <v>41</v>
       </c>
       <c r="F12" s="40">
         <v>3</v>
@@ -2047,16 +1956,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="E13" s="39" t="s">
         <v>43</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="39" t="s">
-        <v>45</v>
       </c>
       <c r="F13" s="40">
         <v>3</v>
@@ -2067,16 +1976,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="E14" s="39" t="s">
         <v>47</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="39" t="s">
-        <v>49</v>
       </c>
       <c r="F14" s="40">
         <v>3</v>
@@ -2087,16 +1996,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D15" s="21" t="s">
         <v>18</v>
       </c>
       <c r="E15" s="39" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F15" s="40">
         <v>3</v>
@@ -2107,16 +2016,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D16" s="21" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="39" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F16" s="40">
         <v>3</v>
@@ -2127,16 +2036,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="41" t="s">
         <v>56</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D17" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="41" t="s">
-        <v>58</v>
       </c>
       <c r="F17" s="42">
         <v>4</v>
@@ -2147,16 +2056,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="E18" s="41" t="s">
         <v>60</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="E18" s="41" t="s">
-        <v>62</v>
       </c>
       <c r="F18" s="42">
         <v>4</v>
@@ -2167,16 +2076,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="E19" s="41" t="s">
         <v>64</v>
-      </c>
-      <c r="D19" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="E19" s="41" t="s">
-        <v>66</v>
       </c>
       <c r="F19" s="42">
         <v>4</v>
@@ -2187,16 +2096,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="E20" s="41" t="s">
         <v>68</v>
-      </c>
-      <c r="D20" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" s="41" t="s">
-        <v>70</v>
       </c>
       <c r="F20" s="42">
         <v>4</v>
@@ -2207,16 +2116,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D21" s="23" t="s">
         <v>18</v>
       </c>
       <c r="E21" s="41" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F21" s="42">
         <v>4</v>
@@ -2227,16 +2136,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="41" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F22" s="42">
         <v>4</v>
@@ -2247,16 +2156,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="E23" s="43" t="s">
         <v>78</v>
-      </c>
-      <c r="D23" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="E23" s="43" t="s">
-        <v>80</v>
       </c>
       <c r="F23" s="3">
         <v>5</v>
@@ -2267,16 +2176,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="E24" s="55" t="s">
         <v>82</v>
-      </c>
-      <c r="D24" s="54" t="s">
-        <v>83</v>
-      </c>
-      <c r="E24" s="55" t="s">
-        <v>84</v>
       </c>
       <c r="F24" s="3">
         <v>5</v>
@@ -2287,16 +2196,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="E25" s="43" t="s">
         <v>86</v>
-      </c>
-      <c r="D25" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="E25" s="43" t="s">
-        <v>88</v>
       </c>
       <c r="F25" s="3">
         <v>5</v>
@@ -2307,16 +2216,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="E26" s="43" t="s">
         <v>89</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D26" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="E26" s="43" t="s">
-        <v>92</v>
       </c>
       <c r="F26" s="3">
         <v>5</v>
@@ -2327,10 +2236,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D27" s="24" t="s">
         <v>8</v>
@@ -2347,16 +2256,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E28" s="43" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F28" s="3">
         <v>5</v>
@@ -2368,16 +2277,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D29" s="25" t="s">
         <v>27</v>
       </c>
       <c r="E29" s="44" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F29" s="45">
         <v>6</v>
@@ -2388,13 +2297,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E30" s="44" t="s">
         <v>15</v>
@@ -2408,16 +2317,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D31" s="25" t="s">
         <v>31</v>
       </c>
       <c r="E31" s="44" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F31" s="45">
         <v>6</v>
@@ -2428,16 +2337,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D32" s="25" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E32" s="44" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F32" s="45">
         <v>6</v>
@@ -2448,10 +2357,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D33" s="25" t="s">
         <v>8</v>
@@ -2468,13 +2377,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D34" s="25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E34" s="44" t="s">
         <v>15</v>
@@ -2488,10 +2397,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D35" s="26" t="s">
         <v>15</v>
@@ -2508,16 +2417,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D36" s="26" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E36" s="46" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="F36" s="47">
         <v>7</v>
@@ -2528,16 +2437,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>121</v>
+        <v>19</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D37" s="26" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="E37" s="46" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F37" s="47">
         <v>7</v>
@@ -2548,16 +2457,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E38" s="46" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F38" s="47">
         <v>7</v>
@@ -2568,10 +2477,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D39" s="26" t="s">
         <v>8</v>
@@ -2588,13 +2497,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="27" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C40" s="27" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D40" s="28" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E40" s="48" t="s">
         <v>15</v>
@@ -2608,13 +2517,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="27" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C41" s="27" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D41" s="28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E41" s="48" t="s">
         <v>15</v>
@@ -2628,13 +2537,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="27" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D42" s="28" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="E42" s="48" t="s">
         <v>15</v>
@@ -2648,16 +2557,16 @@
         <v>42</v>
       </c>
       <c r="B43" s="27" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C43" s="27" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D43" s="28" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E43" s="48" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F43" s="49">
         <v>8</v>
@@ -2668,16 +2577,16 @@
         <v>43</v>
       </c>
       <c r="B44" s="27" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="D44" s="28" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E44" s="48" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F44" s="49">
         <v>8</v>
@@ -2688,10 +2597,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>145</v>
+        <v>61</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D45" s="29" t="s">
         <v>8</v>
@@ -2708,13 +2617,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>147</v>
+        <v>98</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="D46" s="29" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E46" s="50" t="s">
         <v>15</v>
@@ -2728,10 +2637,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>149</v>
+        <v>61</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D47" s="29" t="s">
         <v>8</v>
@@ -2748,13 +2657,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>151</v>
+        <v>98</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="D48" s="29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E48" s="50" t="s">
         <v>15</v>
@@ -2768,13 +2677,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="D49" s="29" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="E49" s="50" t="s">
         <v>15</v>
@@ -2788,10 +2697,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="30" t="s">
-        <v>156</v>
+        <v>61</v>
       </c>
       <c r="C50" s="30" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="D50" s="31" t="s">
         <v>8</v>
@@ -2808,10 +2717,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="30" t="s">
-        <v>158</v>
+        <v>61</v>
       </c>
       <c r="C51" s="30" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="D51" s="31" t="s">
         <v>8</v>
@@ -2828,10 +2737,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="30" t="s">
-        <v>160</v>
+        <v>61</v>
       </c>
       <c r="C52" s="30" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="D52" s="31" t="s">
         <v>8</v>
@@ -2848,10 +2757,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="30" t="s">
-        <v>162</v>
+        <v>61</v>
       </c>
       <c r="C53" s="30" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="D53" s="31" t="s">
         <v>8</v>
@@ -2868,13 +2777,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="30" t="s">
-        <v>164</v>
+        <v>83</v>
       </c>
       <c r="C54" s="30" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="D54" s="31" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E54" s="30" t="s">
         <v>15</v>
@@ -2888,13 +2797,13 @@
         <v>54</v>
       </c>
       <c r="B55" s="32" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="C55" s="32" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="D55" s="33" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="E55" s="32"/>
       <c r="F55" s="32">
@@ -2906,13 +2815,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="32" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="C56" s="32" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="D56" s="33" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="E56" s="32"/>
       <c r="F56" s="32">
@@ -2924,13 +2833,13 @@
         <v>99</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="D57" s="31" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="E57" s="30" t="s">
         <v>8</v>
@@ -2967,22 +2876,22 @@
   <sheetData>
     <row r="2" spans="1:6">
       <c r="A2" s="7" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2990,16 +2899,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="D3" s="11">
         <v>54</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="F3" s="4"/>
     </row>
@@ -3008,16 +2917,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="D4" s="11">
         <v>54</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="F4" s="4"/>
     </row>
@@ -3026,16 +2935,16 @@
         <v>1</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="D5" s="11">
         <v>54</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="F5" s="4"/>
     </row>
@@ -3044,16 +2953,16 @@
         <v>1</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>189</v>
+        <v>132</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
       <c r="D6" s="11">
         <v>54</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="F6" s="4"/>
     </row>
@@ -3062,16 +2971,16 @@
         <v>1</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
       <c r="D7" s="11">
         <v>54</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
       <c r="F7" s="4"/>
     </row>
@@ -3102,18 +3011,18 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>95</v>
+        <v>178</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>195</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="4" t="s">
-        <v>74</v>
+        <v>179</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:2">

</xml_diff>